<commit_message>
fix: rebuilt cosas emx (#3)
</commit_message>
<xml_diff>
--- a/emx/cosas/cosas.xlsx
+++ b/emx/cosas/cosas.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">COSAS</t>
   </si>
   <si>
-    <t xml:space="preserve">The Catalogue of Sequence Array and Samples (v0.9025, 2021-08-30)</t>
+    <t xml:space="preserve">The Catalogue of Sequence Array and Samples (v0.9026, 2021-09-01)</t>
   </si>
   <si>
     <t xml:space="preserve">label-nl</t>
@@ -373,7 +373,7 @@
     <t xml:space="preserve">excludedPhenotypeHpo</t>
   </si>
   <si>
-    <t xml:space="preserve">Excluded Phenotype HPO</t>
+    <t xml:space="preserve">Excluded HPO</t>
   </si>
   <si>
     <t xml:space="preserve">Uitgesloten fenotype HPO</t>
@@ -382,7 +382,7 @@
     <t xml:space="preserve">confirmedPhenotype</t>
   </si>
   <si>
-    <t xml:space="preserve">Confirmed Phenotyp</t>
+    <t xml:space="preserve">Confirmed Phenotype</t>
   </si>
   <si>
     <t xml:space="preserve">Bevestigde Phenotype</t>

</xml_diff>

<commit_message>
fix: added missing timestamp (#3)
</commit_message>
<xml_diff>
--- a/emx/cosas/cosas.xlsx
+++ b/emx/cosas/cosas.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">COSAS</t>
   </si>
   <si>
-    <t xml:space="preserve">The Catalogue of Sequence Array and Samples (v0.9026, 2021-09-01)</t>
+    <t xml:space="preserve">The Catalogue of Sequence Array and Samples (v0.9027, 2021-09-02)</t>
   </si>
   <si>
     <t xml:space="preserve">label-nl</t>
@@ -1831,71 +1831,75 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>96</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="D23" t="s">
-        <v>43</v>
+        <v>98</v>
       </c>
       <c r="E23" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="F23" t="b">
         <v>0</v>
       </c>
       <c r="G23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" t="s">
-        <v>125</v>
-      </c>
-      <c r="I23" t="s">
-        <v>45</v>
-      </c>
-      <c r="J23"/>
+        <v>101</v>
+      </c>
+      <c r="I23"/>
+      <c r="J23" t="s">
+        <v>100</v>
+      </c>
       <c r="K23"/>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24"/>
+        <v>42</v>
+      </c>
+      <c r="D24" t="s">
+        <v>43</v>
+      </c>
       <c r="E24" t="s">
-        <v>44</v>
+        <v>124</v>
       </c>
       <c r="F24" t="b">
         <v>0</v>
       </c>
       <c r="G24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24" t="s">
         <v>125</v>
       </c>
-      <c r="I24"/>
+      <c r="I24" t="s">
+        <v>45</v>
+      </c>
       <c r="J24"/>
       <c r="K24"/>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>126</v>
+        <v>46</v>
       </c>
       <c r="B25" t="s">
-        <v>127</v>
+        <v>47</v>
       </c>
       <c r="C25" t="s">
-        <v>128</v>
+        <v>48</v>
       </c>
       <c r="D25"/>
       <c r="E25" t="s">
@@ -1916,17 +1920,17 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B26" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C26" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D26"/>
       <c r="E26" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="F26" t="b">
         <v>0</v>
@@ -1943,17 +1947,17 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B27" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C27" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D27"/>
       <c r="E27" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="F27" t="b">
         <v>0</v>
@@ -1970,13 +1974,13 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B28" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C28" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D28"/>
       <c r="E28" t="s">
@@ -1997,13 +2001,13 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B29" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C29" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D29"/>
       <c r="E29" t="s">
@@ -2024,17 +2028,17 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B30" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C30" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D30"/>
       <c r="E30" t="s">
-        <v>124</v>
+        <v>44</v>
       </c>
       <c r="F30" t="b">
         <v>0</v>
@@ -2045,21 +2049,19 @@
       <c r="H30" t="s">
         <v>125</v>
       </c>
-      <c r="I30" t="s">
-        <v>144</v>
-      </c>
+      <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B31" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C31" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D31"/>
       <c r="E31" t="s">
@@ -2075,24 +2077,24 @@
         <v>125</v>
       </c>
       <c r="I31" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="J31"/>
       <c r="K31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B32" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C32" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D32"/>
       <c r="E32" t="s">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="F32" t="b">
         <v>0</v>
@@ -2103,23 +2105,25 @@
       <c r="H32" t="s">
         <v>125</v>
       </c>
-      <c r="I32"/>
+      <c r="I32" t="s">
+        <v>147</v>
+      </c>
       <c r="J32"/>
       <c r="K32"/>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B33" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C33" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D33"/>
       <c r="E33" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="F33" t="b">
         <v>0</v>
@@ -2136,17 +2140,17 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B34" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C34" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D34"/>
       <c r="E34" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="F34" t="b">
         <v>0</v>
@@ -2163,13 +2167,13 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B35" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C35" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D35"/>
       <c r="E35" t="s">
@@ -2190,17 +2194,17 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B36" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C36" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D36"/>
       <c r="E36" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="F36" t="b">
         <v>0</v>
@@ -2217,17 +2221,17 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B37" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C37" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D37"/>
       <c r="E37" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="F37" t="b">
         <v>0</v>
@@ -2244,17 +2248,17 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B38" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C38" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D38"/>
       <c r="E38" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="F38" t="b">
         <v>0</v>
@@ -2271,17 +2275,17 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B39" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C39" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D39"/>
       <c r="E39" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="F39" t="b">
         <v>0</v>
@@ -2298,17 +2302,17 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B40" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C40" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D40"/>
       <c r="E40" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="F40" t="b">
         <v>0</v>
@@ -2325,17 +2329,17 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B41" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C41" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D41"/>
       <c r="E41" t="s">
-        <v>83</v>
+        <v>44</v>
       </c>
       <c r="F41" t="b">
         <v>0</v>
@@ -2352,17 +2356,17 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B42" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C42" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D42"/>
       <c r="E42" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="F42" t="b">
         <v>0</v>
@@ -2379,19 +2383,17 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>95</v>
+        <v>178</v>
       </c>
       <c r="B43" t="s">
-        <v>96</v>
+        <v>179</v>
       </c>
       <c r="C43" t="s">
-        <v>97</v>
-      </c>
-      <c r="D43" t="s">
-        <v>98</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="D43"/>
       <c r="E43" t="s">
-        <v>99</v>
+        <v>44</v>
       </c>
       <c r="F43" t="b">
         <v>0</v>
@@ -2403,29 +2405,27 @@
         <v>125</v>
       </c>
       <c r="I43"/>
-      <c r="J43" t="s">
-        <v>100</v>
-      </c>
+      <c r="J43"/>
       <c r="K43"/>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>181</v>
+        <v>95</v>
       </c>
       <c r="B44" t="s">
-        <v>181</v>
+        <v>96</v>
       </c>
       <c r="C44" t="s">
-        <v>181</v>
+        <v>97</v>
       </c>
       <c r="D44" t="s">
-        <v>182</v>
+        <v>98</v>
       </c>
       <c r="E44" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="F44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G44" t="b">
         <v>1</v>
@@ -2435,79 +2435,83 @@
       </c>
       <c r="I44"/>
       <c r="J44" t="s">
-        <v>183</v>
-      </c>
-      <c r="K44" t="b">
-        <v>1</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="K44"/>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>40</v>
+        <v>181</v>
       </c>
       <c r="B45" t="s">
-        <v>41</v>
+        <v>181</v>
       </c>
       <c r="C45" t="s">
-        <v>42</v>
+        <v>181</v>
       </c>
       <c r="D45" t="s">
-        <v>43</v>
+        <v>182</v>
       </c>
       <c r="E45" t="s">
-        <v>124</v>
+        <v>44</v>
       </c>
       <c r="F45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45" t="s">
-        <v>184</v>
-      </c>
-      <c r="I45" t="s">
-        <v>45</v>
-      </c>
-      <c r="J45"/>
-      <c r="K45"/>
+        <v>125</v>
+      </c>
+      <c r="I45"/>
+      <c r="J45" t="s">
+        <v>183</v>
+      </c>
+      <c r="K45" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B46" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C46" t="s">
-        <v>48</v>
-      </c>
-      <c r="D46"/>
+        <v>42</v>
+      </c>
+      <c r="D46" t="s">
+        <v>43</v>
+      </c>
       <c r="E46" t="s">
-        <v>44</v>
+        <v>124</v>
       </c>
       <c r="F46" t="b">
         <v>0</v>
       </c>
       <c r="G46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H46" t="s">
         <v>184</v>
       </c>
-      <c r="I46"/>
+      <c r="I46" t="s">
+        <v>45</v>
+      </c>
       <c r="J46"/>
       <c r="K46"/>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>126</v>
+        <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>127</v>
+        <v>47</v>
       </c>
       <c r="C47" t="s">
-        <v>128</v>
+        <v>48</v>
       </c>
       <c r="D47"/>
       <c r="E47" t="s">
@@ -2528,13 +2532,13 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B48" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C48" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D48"/>
       <c r="E48" t="s">
@@ -2555,17 +2559,17 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B49" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C49" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D49"/>
       <c r="E49" t="s">
-        <v>124</v>
+        <v>44</v>
       </c>
       <c r="F49" t="b">
         <v>0</v>
@@ -2576,25 +2580,23 @@
       <c r="H49" t="s">
         <v>184</v>
       </c>
-      <c r="I49" t="s">
-        <v>144</v>
-      </c>
+      <c r="I49"/>
       <c r="J49"/>
       <c r="K49"/>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>185</v>
+        <v>141</v>
       </c>
       <c r="B50" t="s">
-        <v>186</v>
+        <v>142</v>
       </c>
       <c r="C50" t="s">
-        <v>187</v>
+        <v>143</v>
       </c>
       <c r="D50"/>
       <c r="E50" t="s">
-        <v>44</v>
+        <v>124</v>
       </c>
       <c r="F50" t="b">
         <v>0</v>
@@ -2605,23 +2607,25 @@
       <c r="H50" t="s">
         <v>184</v>
       </c>
-      <c r="I50"/>
+      <c r="I50" t="s">
+        <v>144</v>
+      </c>
       <c r="J50"/>
       <c r="K50"/>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>145</v>
+        <v>185</v>
       </c>
       <c r="B51" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C51" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D51"/>
       <c r="E51" t="s">
-        <v>124</v>
+        <v>44</v>
       </c>
       <c r="F51" t="b">
         <v>0</v>
@@ -2632,25 +2636,23 @@
       <c r="H51" t="s">
         <v>184</v>
       </c>
-      <c r="I51" t="s">
-        <v>147</v>
-      </c>
+      <c r="I51"/>
       <c r="J51"/>
       <c r="K51"/>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B52" t="s">
-        <v>149</v>
+        <v>188</v>
       </c>
       <c r="C52" t="s">
-        <v>150</v>
+        <v>188</v>
       </c>
       <c r="D52"/>
       <c r="E52" t="s">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="F52" t="b">
         <v>0</v>
@@ -2661,25 +2663,25 @@
       <c r="H52" t="s">
         <v>184</v>
       </c>
-      <c r="I52"/>
+      <c r="I52" t="s">
+        <v>147</v>
+      </c>
       <c r="J52"/>
       <c r="K52"/>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>95</v>
+        <v>148</v>
       </c>
       <c r="B53" t="s">
-        <v>96</v>
+        <v>149</v>
       </c>
       <c r="C53" t="s">
-        <v>97</v>
-      </c>
-      <c r="D53" t="s">
-        <v>98</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="D53"/>
       <c r="E53" t="s">
-        <v>99</v>
+        <v>52</v>
       </c>
       <c r="F53" t="b">
         <v>0</v>
@@ -2691,29 +2693,27 @@
         <v>184</v>
       </c>
       <c r="I53"/>
-      <c r="J53" t="s">
-        <v>100</v>
-      </c>
+      <c r="J53"/>
       <c r="K53"/>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>181</v>
+        <v>95</v>
       </c>
       <c r="B54" t="s">
-        <v>181</v>
+        <v>96</v>
       </c>
       <c r="C54" t="s">
-        <v>181</v>
+        <v>97</v>
       </c>
       <c r="D54" t="s">
-        <v>182</v>
+        <v>98</v>
       </c>
       <c r="E54" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="F54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G54" t="b">
         <v>1</v>
@@ -2723,79 +2723,83 @@
       </c>
       <c r="I54"/>
       <c r="J54" t="s">
-        <v>183</v>
-      </c>
-      <c r="K54" t="b">
-        <v>1</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="K54"/>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>40</v>
+        <v>181</v>
       </c>
       <c r="B55" t="s">
-        <v>41</v>
+        <v>181</v>
       </c>
       <c r="C55" t="s">
-        <v>42</v>
+        <v>181</v>
       </c>
       <c r="D55" t="s">
-        <v>43</v>
+        <v>182</v>
       </c>
       <c r="E55" t="s">
-        <v>124</v>
+        <v>44</v>
       </c>
       <c r="F55" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G55" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H55" t="s">
-        <v>189</v>
-      </c>
-      <c r="I55" t="s">
-        <v>45</v>
-      </c>
-      <c r="J55"/>
-      <c r="K55"/>
+        <v>184</v>
+      </c>
+      <c r="I55"/>
+      <c r="J55" t="s">
+        <v>183</v>
+      </c>
+      <c r="K55" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B56" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C56" t="s">
-        <v>48</v>
-      </c>
-      <c r="D56"/>
+        <v>42</v>
+      </c>
+      <c r="D56" t="s">
+        <v>43</v>
+      </c>
       <c r="E56" t="s">
-        <v>44</v>
+        <v>124</v>
       </c>
       <c r="F56" t="b">
         <v>0</v>
       </c>
       <c r="G56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H56" t="s">
         <v>189</v>
       </c>
-      <c r="I56"/>
+      <c r="I56" t="s">
+        <v>45</v>
+      </c>
       <c r="J56"/>
       <c r="K56"/>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>126</v>
+        <v>46</v>
       </c>
       <c r="B57" t="s">
-        <v>127</v>
+        <v>47</v>
       </c>
       <c r="C57" t="s">
-        <v>128</v>
+        <v>48</v>
       </c>
       <c r="D57"/>
       <c r="E57" t="s">
@@ -2816,13 +2820,13 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B58" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C58" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D58"/>
       <c r="E58" t="s">
@@ -2843,17 +2847,17 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B59" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C59" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D59"/>
       <c r="E59" t="s">
-        <v>124</v>
+        <v>44</v>
       </c>
       <c r="F59" t="b">
         <v>0</v>
@@ -2864,25 +2868,23 @@
       <c r="H59" t="s">
         <v>189</v>
       </c>
-      <c r="I59" t="s">
-        <v>144</v>
-      </c>
+      <c r="I59"/>
       <c r="J59"/>
       <c r="K59"/>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>185</v>
+        <v>141</v>
       </c>
       <c r="B60" t="s">
-        <v>186</v>
+        <v>142</v>
       </c>
       <c r="C60" t="s">
-        <v>186</v>
+        <v>143</v>
       </c>
       <c r="D60"/>
       <c r="E60" t="s">
-        <v>44</v>
+        <v>124</v>
       </c>
       <c r="F60" t="b">
         <v>0</v>
@@ -2893,23 +2895,25 @@
       <c r="H60" t="s">
         <v>189</v>
       </c>
-      <c r="I60"/>
+      <c r="I60" t="s">
+        <v>144</v>
+      </c>
       <c r="J60"/>
       <c r="K60"/>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>145</v>
+        <v>185</v>
       </c>
       <c r="B61" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C61" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D61"/>
       <c r="E61" t="s">
-        <v>124</v>
+        <v>44</v>
       </c>
       <c r="F61" t="b">
         <v>0</v>
@@ -2920,25 +2924,23 @@
       <c r="H61" t="s">
         <v>189</v>
       </c>
-      <c r="I61" t="s">
-        <v>147</v>
-      </c>
+      <c r="I61"/>
       <c r="J61"/>
       <c r="K61"/>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B62" t="s">
-        <v>149</v>
+        <v>188</v>
       </c>
       <c r="C62" t="s">
-        <v>150</v>
+        <v>188</v>
       </c>
       <c r="D62"/>
       <c r="E62" t="s">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="F62" t="b">
         <v>0</v>
@@ -2949,23 +2951,25 @@
       <c r="H62" t="s">
         <v>189</v>
       </c>
-      <c r="I62"/>
+      <c r="I62" t="s">
+        <v>147</v>
+      </c>
       <c r="J62"/>
       <c r="K62"/>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>190</v>
+        <v>148</v>
       </c>
       <c r="B63" t="s">
-        <v>191</v>
+        <v>149</v>
       </c>
       <c r="C63" t="s">
-        <v>191</v>
+        <v>150</v>
       </c>
       <c r="D63"/>
       <c r="E63" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="F63" t="b">
         <v>0</v>
@@ -2982,13 +2986,13 @@
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B64" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C64" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D64"/>
       <c r="E64" t="s">
@@ -3009,13 +3013,13 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B65" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C65" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D65"/>
       <c r="E65" t="s">
@@ -3036,13 +3040,13 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B66" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C66" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D66"/>
       <c r="E66" t="s">
@@ -3063,13 +3067,13 @@
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B67" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C67" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D67"/>
       <c r="E67" t="s">
@@ -3090,13 +3094,13 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B68" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C68" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D68"/>
       <c r="E68" t="s">
@@ -3117,13 +3121,13 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B69" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C69" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D69"/>
       <c r="E69" t="s">
@@ -3144,19 +3148,17 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>95</v>
+        <v>204</v>
       </c>
       <c r="B70" t="s">
-        <v>96</v>
+        <v>205</v>
       </c>
       <c r="C70" t="s">
-        <v>97</v>
-      </c>
-      <c r="D70" t="s">
-        <v>98</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="D70"/>
       <c r="E70" t="s">
-        <v>99</v>
+        <v>44</v>
       </c>
       <c r="F70" t="b">
         <v>0</v>
@@ -3168,29 +3170,27 @@
         <v>189</v>
       </c>
       <c r="I70"/>
-      <c r="J70" t="s">
-        <v>100</v>
-      </c>
+      <c r="J70"/>
       <c r="K70"/>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>181</v>
+        <v>95</v>
       </c>
       <c r="B71" t="s">
-        <v>181</v>
+        <v>96</v>
       </c>
       <c r="C71" t="s">
-        <v>181</v>
+        <v>97</v>
       </c>
       <c r="D71" t="s">
-        <v>182</v>
+        <v>98</v>
       </c>
       <c r="E71" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="F71" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G71" t="b">
         <v>1</v>
@@ -3200,79 +3200,83 @@
       </c>
       <c r="I71"/>
       <c r="J71" t="s">
-        <v>183</v>
-      </c>
-      <c r="K71" t="b">
-        <v>1</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="K71"/>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>40</v>
+        <v>181</v>
       </c>
       <c r="B72" t="s">
-        <v>41</v>
+        <v>181</v>
       </c>
       <c r="C72" t="s">
-        <v>42</v>
+        <v>181</v>
       </c>
       <c r="D72" t="s">
-        <v>43</v>
+        <v>182</v>
       </c>
       <c r="E72" t="s">
-        <v>124</v>
+        <v>44</v>
       </c>
       <c r="F72" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G72" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H72" t="s">
-        <v>206</v>
-      </c>
-      <c r="I72" t="s">
-        <v>45</v>
-      </c>
-      <c r="J72"/>
-      <c r="K72"/>
+        <v>189</v>
+      </c>
+      <c r="I72"/>
+      <c r="J72" t="s">
+        <v>183</v>
+      </c>
+      <c r="K72" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B73" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C73" t="s">
-        <v>48</v>
-      </c>
-      <c r="D73"/>
+        <v>42</v>
+      </c>
+      <c r="D73" t="s">
+        <v>43</v>
+      </c>
       <c r="E73" t="s">
-        <v>44</v>
+        <v>124</v>
       </c>
       <c r="F73" t="b">
         <v>0</v>
       </c>
       <c r="G73" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H73" t="s">
         <v>206</v>
       </c>
-      <c r="I73"/>
+      <c r="I73" t="s">
+        <v>45</v>
+      </c>
       <c r="J73"/>
       <c r="K73"/>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>135</v>
+        <v>46</v>
       </c>
       <c r="B74" t="s">
-        <v>136</v>
+        <v>47</v>
       </c>
       <c r="C74" t="s">
-        <v>137</v>
+        <v>48</v>
       </c>
       <c r="D74"/>
       <c r="E74" t="s">
@@ -3293,17 +3297,17 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>185</v>
+        <v>135</v>
       </c>
       <c r="B75" t="s">
-        <v>186</v>
+        <v>136</v>
       </c>
       <c r="C75" t="s">
-        <v>186</v>
+        <v>137</v>
       </c>
       <c r="D75"/>
       <c r="E75" t="s">
-        <v>124</v>
+        <v>44</v>
       </c>
       <c r="F75" t="b">
         <v>0</v>
@@ -3314,25 +3318,23 @@
       <c r="H75" t="s">
         <v>206</v>
       </c>
-      <c r="I75" t="s">
-        <v>147</v>
-      </c>
+      <c r="I75"/>
       <c r="J75"/>
       <c r="K75"/>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="B76" t="s">
-        <v>208</v>
+        <v>186</v>
       </c>
       <c r="C76" t="s">
-        <v>209</v>
+        <v>186</v>
       </c>
       <c r="D76"/>
       <c r="E76" t="s">
-        <v>44</v>
+        <v>124</v>
       </c>
       <c r="F76" t="b">
         <v>0</v>
@@ -3343,19 +3345,21 @@
       <c r="H76" t="s">
         <v>206</v>
       </c>
-      <c r="I76"/>
+      <c r="I76" t="s">
+        <v>147</v>
+      </c>
       <c r="J76"/>
       <c r="K76"/>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B77" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C77" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D77"/>
       <c r="E77" t="s">
@@ -3376,13 +3380,13 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B78" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C78" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D78"/>
       <c r="E78" t="s">
@@ -3403,13 +3407,13 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B79" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C79" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D79"/>
       <c r="E79" t="s">
@@ -3430,17 +3434,17 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B80" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C80" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D80"/>
       <c r="E80" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="F80" t="b">
         <v>0</v>
@@ -3457,19 +3461,17 @@
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>95</v>
+        <v>215</v>
       </c>
       <c r="B81" t="s">
-        <v>96</v>
+        <v>216</v>
       </c>
       <c r="C81" t="s">
-        <v>97</v>
-      </c>
-      <c r="D81" t="s">
-        <v>98</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="D81"/>
       <c r="E81" t="s">
-        <v>99</v>
+        <v>52</v>
       </c>
       <c r="F81" t="b">
         <v>0</v>
@@ -3481,29 +3483,27 @@
         <v>206</v>
       </c>
       <c r="I81"/>
-      <c r="J81" t="s">
-        <v>100</v>
-      </c>
+      <c r="J81"/>
       <c r="K81"/>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>181</v>
+        <v>95</v>
       </c>
       <c r="B82" t="s">
-        <v>181</v>
+        <v>96</v>
       </c>
       <c r="C82" t="s">
-        <v>181</v>
+        <v>97</v>
       </c>
       <c r="D82" t="s">
-        <v>182</v>
+        <v>98</v>
       </c>
       <c r="E82" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="F82" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G82" t="b">
         <v>1</v>
@@ -3513,9 +3513,40 @@
       </c>
       <c r="I82"/>
       <c r="J82" t="s">
+        <v>100</v>
+      </c>
+      <c r="K82"/>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>181</v>
+      </c>
+      <c r="B83" t="s">
+        <v>181</v>
+      </c>
+      <c r="C83" t="s">
+        <v>181</v>
+      </c>
+      <c r="D83" t="s">
+        <v>182</v>
+      </c>
+      <c r="E83" t="s">
+        <v>44</v>
+      </c>
+      <c r="F83" t="b">
+        <v>1</v>
+      </c>
+      <c r="G83" t="b">
+        <v>1</v>
+      </c>
+      <c r="H83" t="s">
+        <v>206</v>
+      </c>
+      <c r="I83"/>
+      <c r="J83" t="s">
         <v>183</v>
       </c>
-      <c r="K82" t="b">
+      <c r="K83" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>